<commit_message>
utilizzo della libreria accell stepper
</commit_message>
<xml_diff>
--- a/Control/Parts_Information.xlsx
+++ b/Control/Parts_Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Documents\Nyrio_Software\Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC316EC-351E-489E-91B4-8AC0A363FEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6FE2F1-0092-47EF-A909-5155C7CA6A3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{AE5F5D6C-6889-4F63-8296-C1BE80BF43D0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Pezzo</t>
   </si>
@@ -194,8 +194,8 @@
   <autoFilter ref="A1:D19" xr:uid="{7C98465A-C75F-41BF-AD02-6AB0385669F9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C59CAD38-2C64-46A3-A7D3-1C580F013A66}" name="Pezzo"/>
-    <tableColumn id="2" xr3:uid="{0E18D62A-74BF-43D9-A59E-FAD2F81B6642}" name="Peso (gr)" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{B5C9407F-C96A-450E-91ED-ED710CEE7972}" name="Available" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{0E18D62A-74BF-43D9-A59E-FAD2F81B6642}" name="Peso (gr)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B5C9407F-C96A-450E-91ED-ED710CEE7972}" name="Available" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{2B49B73B-83ED-4D8C-8693-9B9209C7795D}" name="Baricentro(xyz)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -575,7 +575,9 @@
       <c r="B6" s="2">
         <v>210</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">

</xml_diff>